<commit_message>
import correctly all data. enable light simulation
</commit_message>
<xml_diff>
--- a/data/capteur.xlsx
+++ b/data/capteur.xlsx
@@ -1,18 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10513"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stahl\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fboudon/Develop/oagit/mangolight/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{DFF78B0C-DB5C-C449-8FB0-B2047D4BF64A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11505" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19620" windowHeight="14240" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
+    <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000"/>
   <extLst>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="77">
   <si>
     <t>UC</t>
   </si>
@@ -72,13 +75,196 @@
   </si>
   <si>
     <t>slow (2,72ms)</t>
+  </si>
+  <si>
+    <t>Topo</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Diam</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Id_isa</t>
+  </si>
+  <si>
+    <t>*^/A1/S1</t>
+  </si>
+  <si>
+    <t>*^&lt;S2</t>
+  </si>
+  <si>
+    <t>*^&lt;S3</t>
+  </si>
+  <si>
+    <t>3B1</t>
+  </si>
+  <si>
+    <t>*^&lt;S4</t>
+  </si>
+  <si>
+    <t>*^&lt;S5</t>
+  </si>
+  <si>
+    <t>*^&lt;S6</t>
+  </si>
+  <si>
+    <t>*^&lt;S7</t>
+  </si>
+  <si>
+    <t>*^&lt;S8</t>
+  </si>
+  <si>
+    <t>*^&lt;S9</t>
+  </si>
+  <si>
+    <t>*^&lt;S10</t>
+  </si>
+  <si>
+    <t>*^&lt;S11</t>
+  </si>
+  <si>
+    <t>*^&lt;S12</t>
+  </si>
+  <si>
+    <t>*^&lt;S13</t>
+  </si>
+  <si>
+    <t>*^&lt;S14</t>
+  </si>
+  <si>
+    <t>*^&lt;S15</t>
+  </si>
+  <si>
+    <t>*^&lt;S16</t>
+  </si>
+  <si>
+    <t>*^&lt;S17</t>
+  </si>
+  <si>
+    <t>*^&lt;S18</t>
+  </si>
+  <si>
+    <t>*^&lt;S19</t>
+  </si>
+  <si>
+    <t>*^&lt;S20</t>
+  </si>
+  <si>
+    <t>*^&lt;S21</t>
+  </si>
+  <si>
+    <t>*^&lt;S22</t>
+  </si>
+  <si>
+    <t>*^&lt;S23</t>
+  </si>
+  <si>
+    <t>*^&lt;S24</t>
+  </si>
+  <si>
+    <t>*^&lt;S25</t>
+  </si>
+  <si>
+    <t>*^&lt;S26</t>
+  </si>
+  <si>
+    <t>*^&lt;S27</t>
+  </si>
+  <si>
+    <t>*^&lt;S28</t>
+  </si>
+  <si>
+    <t>*^&lt;S29</t>
+  </si>
+  <si>
+    <t>*^&lt;S30</t>
+  </si>
+  <si>
+    <t>*^&lt;S31</t>
+  </si>
+  <si>
+    <t>*^&lt;S32</t>
+  </si>
+  <si>
+    <t>*^&lt;S33</t>
+  </si>
+  <si>
+    <t>*^&lt;S34</t>
+  </si>
+  <si>
+    <t>*^&lt;S35</t>
+  </si>
+  <si>
+    <t>*^&lt;S36</t>
+  </si>
+  <si>
+    <t>*^&lt;S37</t>
+  </si>
+  <si>
+    <t>*^&lt;S38</t>
+  </si>
+  <si>
+    <t>*^&lt;S39</t>
+  </si>
+  <si>
+    <t>*^&lt;S40</t>
+  </si>
+  <si>
+    <t>*^&lt;S41</t>
+  </si>
+  <si>
+    <t>*^&lt;S42</t>
+  </si>
+  <si>
+    <t>*^&lt;S43</t>
+  </si>
+  <si>
+    <t>*^&lt;S44</t>
+  </si>
+  <si>
+    <t>*^&lt;S45</t>
+  </si>
+  <si>
+    <t>*^&lt;S46</t>
+  </si>
+  <si>
+    <t>*^&lt;S47</t>
+  </si>
+  <si>
+    <t>*^&lt;S48</t>
+  </si>
+  <si>
+    <t>*^&lt;S49</t>
+  </si>
+  <si>
+    <t>*^&lt;S50</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -91,6 +277,34 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF00FF00"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF00FF00"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -128,7 +342,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -140,6 +354,10 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -478,21 +696,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" style="3" customWidth="1"/>
     <col min="2" max="2" width="28.5" style="3" customWidth="1"/>
-    <col min="3" max="3" width="31.875" customWidth="1"/>
+    <col min="3" max="3" width="31.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -503,7 +721,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -514,7 +732,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -525,7 +743,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -536,7 +754,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -547,7 +765,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -558,7 +776,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -569,7 +787,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -580,7 +798,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -591,7 +809,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -602,7 +820,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -613,7 +831,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -624,7 +842,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -635,7 +853,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -646,7 +864,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -657,7 +875,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -668,7 +886,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -679,7 +897,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -690,7 +908,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -701,7 +919,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -712,7 +930,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -723,7 +941,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -734,7 +952,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -745,7 +963,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -756,7 +974,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -767,7 +985,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -778,7 +996,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -789,7 +1007,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -800,7 +1018,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -811,7 +1029,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -822,7 +1040,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -833,7 +1051,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -844,7 +1062,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -855,7 +1073,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>10</v>
       </c>
@@ -863,22 +1081,22 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B36" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B37" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B38" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B39" s="3" t="s">
         <v>15</v>
       </c>
@@ -893,4 +1111,2229 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7460550-1CCA-CD43-BF8F-3E8D58EBE9C7}">
+  <dimension ref="A1:J51"/>
+  <sheetViews>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="5">
+        <v>64.69</v>
+      </c>
+      <c r="C2" s="5">
+        <v>3.41</v>
+      </c>
+      <c r="D2" s="5">
+        <v>-82.7</v>
+      </c>
+      <c r="E2" s="5">
+        <v>-49.54</v>
+      </c>
+      <c r="F2" s="5">
+        <v>10.4</v>
+      </c>
+      <c r="G2" s="5">
+        <v>-18.739999999999998</v>
+      </c>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="6"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="5">
+        <v>33.67</v>
+      </c>
+      <c r="C3" s="5">
+        <v>-41.91</v>
+      </c>
+      <c r="D3" s="5">
+        <v>-82.24</v>
+      </c>
+      <c r="E3" s="5">
+        <v>-87.32</v>
+      </c>
+      <c r="F3" s="5">
+        <v>9.43</v>
+      </c>
+      <c r="G3" s="5">
+        <v>-48.49</v>
+      </c>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="6"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="5">
+        <v>-8.5</v>
+      </c>
+      <c r="C4" s="5">
+        <v>31.97</v>
+      </c>
+      <c r="D4" s="5">
+        <v>-164.52</v>
+      </c>
+      <c r="E4" s="5">
+        <v>124.25</v>
+      </c>
+      <c r="F4" s="5">
+        <v>-5.97</v>
+      </c>
+      <c r="G4" s="5">
+        <v>6.23</v>
+      </c>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="6"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="5">
+        <v>-148.68</v>
+      </c>
+      <c r="C5" s="5">
+        <v>93.5</v>
+      </c>
+      <c r="D5" s="5">
+        <v>-133.16999999999999</v>
+      </c>
+      <c r="E5" s="5">
+        <v>-77.209999999999994</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0.67</v>
+      </c>
+      <c r="G5" s="5">
+        <v>5.22</v>
+      </c>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6">
+        <v>1</v>
+      </c>
+      <c r="J5" s="6"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="5">
+        <v>-136.71</v>
+      </c>
+      <c r="C6" s="5">
+        <v>62.2</v>
+      </c>
+      <c r="D6" s="5">
+        <v>-139.68</v>
+      </c>
+      <c r="E6" s="5">
+        <v>-172.53</v>
+      </c>
+      <c r="F6" s="5">
+        <v>-1.94</v>
+      </c>
+      <c r="G6" s="5">
+        <v>15.11</v>
+      </c>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6">
+        <v>2</v>
+      </c>
+      <c r="J6" s="6">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="5">
+        <v>-111.26</v>
+      </c>
+      <c r="C7" s="5">
+        <v>25.89</v>
+      </c>
+      <c r="D7" s="5">
+        <v>-135.47999999999999</v>
+      </c>
+      <c r="E7" s="5">
+        <v>173.51</v>
+      </c>
+      <c r="F7" s="5">
+        <v>-19.100000000000001</v>
+      </c>
+      <c r="G7" s="5">
+        <v>23.12</v>
+      </c>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6">
+        <v>3</v>
+      </c>
+      <c r="J7" s="6"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="5">
+        <v>53.07</v>
+      </c>
+      <c r="C8" s="5">
+        <v>-293.66000000000003</v>
+      </c>
+      <c r="D8" s="5">
+        <v>35.96</v>
+      </c>
+      <c r="E8" s="5">
+        <v>-118.85</v>
+      </c>
+      <c r="F8" s="5">
+        <v>-17.91</v>
+      </c>
+      <c r="G8" s="5">
+        <v>-10.69</v>
+      </c>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6">
+        <v>110</v>
+      </c>
+      <c r="J8" s="6"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="5">
+        <v>69.37</v>
+      </c>
+      <c r="C9" s="5">
+        <v>-270.64999999999998</v>
+      </c>
+      <c r="D9" s="5">
+        <v>38.909999999999997</v>
+      </c>
+      <c r="E9" s="5">
+        <v>-102.11</v>
+      </c>
+      <c r="F9" s="5">
+        <v>-50.35</v>
+      </c>
+      <c r="G9" s="5">
+        <v>-28.07</v>
+      </c>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6">
+        <v>111</v>
+      </c>
+      <c r="J9" s="6"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="5">
+        <v>75.77</v>
+      </c>
+      <c r="C10" s="5">
+        <v>-212.1</v>
+      </c>
+      <c r="D10" s="5">
+        <v>53.71</v>
+      </c>
+      <c r="E10" s="5">
+        <v>105.88</v>
+      </c>
+      <c r="F10" s="5">
+        <v>-46.01</v>
+      </c>
+      <c r="G10" s="5">
+        <v>3.19</v>
+      </c>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6">
+        <v>112</v>
+      </c>
+      <c r="J10" s="6"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="5">
+        <v>117.51</v>
+      </c>
+      <c r="C11" s="5">
+        <v>74.08</v>
+      </c>
+      <c r="D11" s="5">
+        <v>-147.46</v>
+      </c>
+      <c r="E11" s="5">
+        <v>-18.75</v>
+      </c>
+      <c r="F11" s="5">
+        <v>1.48</v>
+      </c>
+      <c r="G11" s="5">
+        <v>-6.03</v>
+      </c>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6">
+        <v>32</v>
+      </c>
+      <c r="J11" s="6"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="5">
+        <v>55.85</v>
+      </c>
+      <c r="C12" s="5">
+        <v>-49.81</v>
+      </c>
+      <c r="D12" s="5">
+        <v>-150.11000000000001</v>
+      </c>
+      <c r="E12" s="5">
+        <v>-92.66</v>
+      </c>
+      <c r="F12" s="5">
+        <v>-1.79</v>
+      </c>
+      <c r="G12" s="5">
+        <v>-7.98</v>
+      </c>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6">
+        <v>30</v>
+      </c>
+      <c r="J12" s="6"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="5">
+        <v>-40.53</v>
+      </c>
+      <c r="C13" s="5">
+        <v>-86.38</v>
+      </c>
+      <c r="D13" s="5">
+        <v>-158.86000000000001</v>
+      </c>
+      <c r="E13" s="5">
+        <v>-76.25</v>
+      </c>
+      <c r="F13" s="5">
+        <v>-12.15</v>
+      </c>
+      <c r="G13" s="5">
+        <v>19.14</v>
+      </c>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6">
+        <v>29</v>
+      </c>
+      <c r="J13" s="6"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="5">
+        <v>-27.09</v>
+      </c>
+      <c r="C14" s="5">
+        <v>-2.62</v>
+      </c>
+      <c r="D14" s="5">
+        <v>-83.24</v>
+      </c>
+      <c r="E14" s="5">
+        <v>-61.45</v>
+      </c>
+      <c r="F14" s="5">
+        <v>-2.58</v>
+      </c>
+      <c r="G14" s="5">
+        <v>7.08</v>
+      </c>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6">
+        <v>31</v>
+      </c>
+      <c r="J14" s="6"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="5">
+        <v>70.14</v>
+      </c>
+      <c r="C15" s="5">
+        <v>-224.82</v>
+      </c>
+      <c r="D15" s="5">
+        <v>-149.83000000000001</v>
+      </c>
+      <c r="E15" s="5">
+        <v>62.09</v>
+      </c>
+      <c r="F15" s="5">
+        <v>-25.8</v>
+      </c>
+      <c r="G15" s="5">
+        <v>-20.58</v>
+      </c>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6">
+        <v>4</v>
+      </c>
+      <c r="J15" s="6"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="5">
+        <v>76.08</v>
+      </c>
+      <c r="C16" s="5">
+        <v>-191.77</v>
+      </c>
+      <c r="D16" s="5">
+        <v>-150.53</v>
+      </c>
+      <c r="E16" s="5">
+        <v>6.23</v>
+      </c>
+      <c r="F16" s="5">
+        <v>-13.09</v>
+      </c>
+      <c r="G16" s="5">
+        <v>12.68</v>
+      </c>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6">
+        <v>5</v>
+      </c>
+      <c r="J16" s="6"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="5">
+        <v>76.66</v>
+      </c>
+      <c r="C17" s="5">
+        <v>-146.81</v>
+      </c>
+      <c r="D17" s="5">
+        <v>-190.99</v>
+      </c>
+      <c r="E17" s="5">
+        <v>37.21</v>
+      </c>
+      <c r="F17" s="5">
+        <v>17.940000000000001</v>
+      </c>
+      <c r="G17" s="5">
+        <v>8.6199999999999992</v>
+      </c>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6">
+        <v>6</v>
+      </c>
+      <c r="J17" s="6"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="5">
+        <v>238.33</v>
+      </c>
+      <c r="C18" s="5">
+        <v>-31.44</v>
+      </c>
+      <c r="D18" s="5">
+        <v>-127.51</v>
+      </c>
+      <c r="E18" s="5">
+        <v>85.31</v>
+      </c>
+      <c r="F18" s="5">
+        <v>-34.950000000000003</v>
+      </c>
+      <c r="G18" s="5">
+        <v>9.15</v>
+      </c>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6">
+        <v>7</v>
+      </c>
+      <c r="J18" s="6"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="5">
+        <v>216.7</v>
+      </c>
+      <c r="C19" s="5">
+        <v>-4.54</v>
+      </c>
+      <c r="D19" s="5">
+        <v>-132.74</v>
+      </c>
+      <c r="E19" s="5">
+        <v>12.38</v>
+      </c>
+      <c r="F19" s="5">
+        <v>-28.66</v>
+      </c>
+      <c r="G19" s="5">
+        <v>9.86</v>
+      </c>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6">
+        <v>8</v>
+      </c>
+      <c r="J19" s="6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="5">
+        <v>208.77</v>
+      </c>
+      <c r="C20" s="5">
+        <v>27.35</v>
+      </c>
+      <c r="D20" s="5">
+        <v>-123.77</v>
+      </c>
+      <c r="E20" s="5">
+        <v>25.46</v>
+      </c>
+      <c r="F20" s="5">
+        <v>-22.29</v>
+      </c>
+      <c r="G20" s="5">
+        <v>13.75</v>
+      </c>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6">
+        <v>9</v>
+      </c>
+      <c r="J20" s="6"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="5">
+        <v>-183.67</v>
+      </c>
+      <c r="C21" s="5">
+        <v>48.72</v>
+      </c>
+      <c r="D21" s="5">
+        <v>-265.25</v>
+      </c>
+      <c r="E21" s="5">
+        <v>-39.49</v>
+      </c>
+      <c r="F21" s="5">
+        <v>22.08</v>
+      </c>
+      <c r="G21" s="5">
+        <v>-29.72</v>
+      </c>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6">
+        <v>13</v>
+      </c>
+      <c r="J21" s="6"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="5">
+        <v>-169.91</v>
+      </c>
+      <c r="C22" s="5">
+        <v>28.97</v>
+      </c>
+      <c r="D22" s="5">
+        <v>-261.47000000000003</v>
+      </c>
+      <c r="E22" s="5">
+        <v>55.1</v>
+      </c>
+      <c r="F22" s="5">
+        <v>26.44</v>
+      </c>
+      <c r="G22" s="5">
+        <v>-64.989999999999995</v>
+      </c>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6">
+        <v>14</v>
+      </c>
+      <c r="J22" s="6"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="5">
+        <v>-157.80000000000001</v>
+      </c>
+      <c r="C23" s="5">
+        <v>11.3</v>
+      </c>
+      <c r="D23" s="5">
+        <v>-239.41</v>
+      </c>
+      <c r="E23" s="5">
+        <v>-46.93</v>
+      </c>
+      <c r="F23" s="5">
+        <v>21.62</v>
+      </c>
+      <c r="G23" s="5">
+        <v>-66.41</v>
+      </c>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6">
+        <v>15</v>
+      </c>
+      <c r="J23" s="6"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="5">
+        <v>67.16</v>
+      </c>
+      <c r="C24" s="5">
+        <v>-219.92</v>
+      </c>
+      <c r="D24" s="5">
+        <v>-302.11</v>
+      </c>
+      <c r="E24" s="5">
+        <v>61.3</v>
+      </c>
+      <c r="F24" s="5">
+        <v>-18.25</v>
+      </c>
+      <c r="G24" s="5">
+        <v>-3.52</v>
+      </c>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6">
+        <v>16</v>
+      </c>
+      <c r="J24" s="6"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="5">
+        <v>53.41</v>
+      </c>
+      <c r="C25" s="5">
+        <v>-208.55</v>
+      </c>
+      <c r="D25" s="5">
+        <v>-273.39999999999998</v>
+      </c>
+      <c r="E25" s="5">
+        <v>27.69</v>
+      </c>
+      <c r="F25" s="5">
+        <v>-4.13</v>
+      </c>
+      <c r="G25" s="5">
+        <v>38.74</v>
+      </c>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6">
+        <v>17</v>
+      </c>
+      <c r="J25" s="6"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="5">
+        <v>48.41</v>
+      </c>
+      <c r="C26" s="5">
+        <v>-179.83</v>
+      </c>
+      <c r="D26" s="5">
+        <v>-248.37</v>
+      </c>
+      <c r="E26" s="5">
+        <v>47.35</v>
+      </c>
+      <c r="F26" s="5">
+        <v>-10.16</v>
+      </c>
+      <c r="G26" s="5">
+        <v>53.29</v>
+      </c>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6">
+        <v>18</v>
+      </c>
+      <c r="J26" s="6"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="5">
+        <v>248.64</v>
+      </c>
+      <c r="C27" s="5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D27" s="5">
+        <v>-301.52999999999997</v>
+      </c>
+      <c r="E27" s="5">
+        <v>96.66</v>
+      </c>
+      <c r="F27" s="5">
+        <v>7.09</v>
+      </c>
+      <c r="G27" s="5">
+        <v>-21.65</v>
+      </c>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6">
+        <v>19</v>
+      </c>
+      <c r="J27" s="6"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="5">
+        <v>229.51</v>
+      </c>
+      <c r="C28" s="5">
+        <v>9.09</v>
+      </c>
+      <c r="D28" s="5">
+        <v>-281.70999999999998</v>
+      </c>
+      <c r="E28" s="5">
+        <v>60.22</v>
+      </c>
+      <c r="F28" s="5">
+        <v>37.81</v>
+      </c>
+      <c r="G28" s="5">
+        <v>28.51</v>
+      </c>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6">
+        <v>20</v>
+      </c>
+      <c r="J28" s="6"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" s="5">
+        <v>217.99</v>
+      </c>
+      <c r="C29" s="5">
+        <v>32.76</v>
+      </c>
+      <c r="D29" s="5">
+        <v>-251.13</v>
+      </c>
+      <c r="E29" s="5">
+        <v>87.09</v>
+      </c>
+      <c r="F29" s="5">
+        <v>10.65</v>
+      </c>
+      <c r="G29" s="5">
+        <v>50.39</v>
+      </c>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6">
+        <v>21</v>
+      </c>
+      <c r="J29" s="6"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" s="5">
+        <v>93.07</v>
+      </c>
+      <c r="C30" s="5">
+        <v>141.38</v>
+      </c>
+      <c r="D30" s="5">
+        <v>-311</v>
+      </c>
+      <c r="E30" s="5">
+        <v>-103.6</v>
+      </c>
+      <c r="F30" s="5">
+        <v>4.04</v>
+      </c>
+      <c r="G30" s="5">
+        <v>-75.38</v>
+      </c>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6">
+        <v>22</v>
+      </c>
+      <c r="J30" s="6"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31" s="5">
+        <v>94.18</v>
+      </c>
+      <c r="C31" s="5">
+        <v>118.69</v>
+      </c>
+      <c r="D31" s="5">
+        <v>-279.89</v>
+      </c>
+      <c r="E31" s="5">
+        <v>-95.9</v>
+      </c>
+      <c r="F31" s="5">
+        <v>1.9</v>
+      </c>
+      <c r="G31" s="5">
+        <v>-89.9</v>
+      </c>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6">
+        <v>23</v>
+      </c>
+      <c r="J31" s="6"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B32" s="5">
+        <v>99.21</v>
+      </c>
+      <c r="C32" s="5">
+        <v>104.96</v>
+      </c>
+      <c r="D32" s="5">
+        <v>-239.65</v>
+      </c>
+      <c r="E32" s="5">
+        <v>-96.93</v>
+      </c>
+      <c r="F32" s="5">
+        <v>32</v>
+      </c>
+      <c r="G32" s="5">
+        <v>-3.63</v>
+      </c>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6">
+        <v>24</v>
+      </c>
+      <c r="J32" s="6"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B33" s="5">
+        <v>-46.53</v>
+      </c>
+      <c r="C33" s="5">
+        <v>-18.09</v>
+      </c>
+      <c r="D33" s="5">
+        <v>-265.7</v>
+      </c>
+      <c r="E33" s="5">
+        <v>52.35</v>
+      </c>
+      <c r="F33" s="5">
+        <v>6.85</v>
+      </c>
+      <c r="G33" s="5">
+        <v>5.86</v>
+      </c>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6">
+        <v>28</v>
+      </c>
+      <c r="J33" s="6"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B34" s="5">
+        <v>11.54</v>
+      </c>
+      <c r="C34" s="5">
+        <v>-116.62</v>
+      </c>
+      <c r="D34" s="5">
+        <v>-287.73</v>
+      </c>
+      <c r="E34" s="5">
+        <v>-78.83</v>
+      </c>
+      <c r="F34" s="5">
+        <v>32.49</v>
+      </c>
+      <c r="G34" s="5">
+        <v>67.95</v>
+      </c>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6">
+        <v>27</v>
+      </c>
+      <c r="J34" s="6"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B35" s="5">
+        <v>-22.27</v>
+      </c>
+      <c r="C35" s="5">
+        <v>-64.540000000000006</v>
+      </c>
+      <c r="D35" s="5">
+        <v>-347.43</v>
+      </c>
+      <c r="E35" s="5">
+        <v>-123.15</v>
+      </c>
+      <c r="F35" s="5">
+        <v>49.15</v>
+      </c>
+      <c r="G35" s="5">
+        <v>35.21</v>
+      </c>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6">
+        <v>25</v>
+      </c>
+      <c r="J35" s="6"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B36" s="5">
+        <v>26.39</v>
+      </c>
+      <c r="C36" s="5">
+        <v>-56.61</v>
+      </c>
+      <c r="D36" s="5">
+        <v>-332</v>
+      </c>
+      <c r="E36" s="5">
+        <v>-22.81</v>
+      </c>
+      <c r="F36" s="5">
+        <v>47.63</v>
+      </c>
+      <c r="G36" s="5">
+        <v>75.06</v>
+      </c>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6">
+        <v>26</v>
+      </c>
+      <c r="J36" s="6"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B37" s="5">
+        <v>-158.83000000000001</v>
+      </c>
+      <c r="C37" s="5">
+        <v>-113.65</v>
+      </c>
+      <c r="D37" s="5">
+        <v>-161.57</v>
+      </c>
+      <c r="E37" s="5">
+        <v>26.69</v>
+      </c>
+      <c r="F37" s="5">
+        <v>21.17</v>
+      </c>
+      <c r="G37" s="5">
+        <v>-93.87</v>
+      </c>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="6">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B38" s="5">
+        <v>2.56</v>
+      </c>
+      <c r="C38" s="5">
+        <v>-226.6</v>
+      </c>
+      <c r="D38" s="5">
+        <v>-224.59</v>
+      </c>
+      <c r="E38" s="5">
+        <v>-15.81</v>
+      </c>
+      <c r="F38" s="5">
+        <v>78.58</v>
+      </c>
+      <c r="G38" s="5">
+        <v>-82.38</v>
+      </c>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B39" s="5">
+        <v>131.97999999999999</v>
+      </c>
+      <c r="C39" s="5">
+        <v>-139.75</v>
+      </c>
+      <c r="D39" s="5">
+        <v>-154.04</v>
+      </c>
+      <c r="E39" s="5">
+        <v>133.51</v>
+      </c>
+      <c r="F39" s="5">
+        <v>34.65</v>
+      </c>
+      <c r="G39" s="5">
+        <v>-31.93</v>
+      </c>
+      <c r="H39" s="6"/>
+      <c r="I39" s="6"/>
+      <c r="J39" s="6">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B40" s="5">
+        <v>88.62</v>
+      </c>
+      <c r="C40" s="5">
+        <v>-181.55</v>
+      </c>
+      <c r="D40" s="5">
+        <v>-159.72999999999999</v>
+      </c>
+      <c r="E40" s="5">
+        <v>-174.2</v>
+      </c>
+      <c r="F40" s="5">
+        <v>37</v>
+      </c>
+      <c r="G40" s="5">
+        <v>13.06</v>
+      </c>
+      <c r="H40" s="6"/>
+      <c r="I40" s="6"/>
+      <c r="J40" s="6">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B41" s="5">
+        <v>83.54</v>
+      </c>
+      <c r="C41" s="5">
+        <v>-151.57</v>
+      </c>
+      <c r="D41" s="5">
+        <v>-184.85</v>
+      </c>
+      <c r="E41" s="5">
+        <v>147.93</v>
+      </c>
+      <c r="F41" s="5">
+        <v>-6.3</v>
+      </c>
+      <c r="G41" s="5">
+        <v>-106</v>
+      </c>
+      <c r="H41" s="6"/>
+      <c r="I41" s="6"/>
+      <c r="J41" s="6">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A42" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B42" s="5">
+        <v>37.880000000000003</v>
+      </c>
+      <c r="C42" s="5">
+        <v>199.96</v>
+      </c>
+      <c r="D42" s="5">
+        <v>-217.14</v>
+      </c>
+      <c r="E42" s="5">
+        <v>-110.06</v>
+      </c>
+      <c r="F42" s="5">
+        <v>52.65</v>
+      </c>
+      <c r="G42" s="5">
+        <v>-15.87</v>
+      </c>
+      <c r="H42" s="6"/>
+      <c r="I42" s="6"/>
+      <c r="J42" s="6">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A43" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B43" s="5">
+        <v>-7.56</v>
+      </c>
+      <c r="C43" s="5">
+        <v>188.88</v>
+      </c>
+      <c r="D43" s="5">
+        <v>-193.8</v>
+      </c>
+      <c r="E43" s="5">
+        <v>-76.12</v>
+      </c>
+      <c r="F43" s="5">
+        <v>26.58</v>
+      </c>
+      <c r="G43" s="5">
+        <v>-60.51</v>
+      </c>
+      <c r="H43" s="6"/>
+      <c r="I43" s="6"/>
+      <c r="J43" s="6">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A44" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B44" s="5">
+        <v>218.81</v>
+      </c>
+      <c r="C44" s="5">
+        <v>53.23</v>
+      </c>
+      <c r="D44" s="5">
+        <v>-147.55000000000001</v>
+      </c>
+      <c r="E44" s="5">
+        <v>-118.86</v>
+      </c>
+      <c r="F44" s="5">
+        <v>21.09</v>
+      </c>
+      <c r="G44" s="5">
+        <v>-31.49</v>
+      </c>
+      <c r="H44" s="6"/>
+      <c r="I44" s="6"/>
+      <c r="J44" s="6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B45" s="5">
+        <v>234.64</v>
+      </c>
+      <c r="C45" s="5">
+        <v>40.89</v>
+      </c>
+      <c r="D45" s="5">
+        <v>-182.84</v>
+      </c>
+      <c r="E45" s="5">
+        <v>-131.28</v>
+      </c>
+      <c r="F45" s="5">
+        <v>42.41</v>
+      </c>
+      <c r="G45" s="5">
+        <v>-23.26</v>
+      </c>
+      <c r="H45" s="6"/>
+      <c r="I45" s="6"/>
+      <c r="J45" s="6">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A46" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B46" s="5">
+        <v>83.84</v>
+      </c>
+      <c r="C46" s="5">
+        <v>185.97</v>
+      </c>
+      <c r="D46" s="5">
+        <v>-151.76</v>
+      </c>
+      <c r="E46" s="5">
+        <v>-106.02</v>
+      </c>
+      <c r="F46" s="5">
+        <v>-15.39</v>
+      </c>
+      <c r="G46" s="5">
+        <v>7.12</v>
+      </c>
+      <c r="H46" s="6"/>
+      <c r="I46" s="6">
+        <v>10</v>
+      </c>
+      <c r="J46" s="6"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A47" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B47" s="5">
+        <v>73.69</v>
+      </c>
+      <c r="C47" s="5">
+        <v>163.27000000000001</v>
+      </c>
+      <c r="D47" s="5">
+        <v>-149.35</v>
+      </c>
+      <c r="E47" s="5">
+        <v>-48.95</v>
+      </c>
+      <c r="F47" s="5">
+        <v>-55.5</v>
+      </c>
+      <c r="G47" s="5">
+        <v>-15.03</v>
+      </c>
+      <c r="H47" s="6"/>
+      <c r="I47" s="6">
+        <v>11</v>
+      </c>
+      <c r="J47" s="6"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A48" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B48" s="5">
+        <v>65.7</v>
+      </c>
+      <c r="C48" s="5">
+        <v>123.31</v>
+      </c>
+      <c r="D48" s="5">
+        <v>-164.55</v>
+      </c>
+      <c r="E48" s="5">
+        <v>-27.61</v>
+      </c>
+      <c r="F48" s="5">
+        <v>12.99</v>
+      </c>
+      <c r="G48" s="5">
+        <v>-19.37</v>
+      </c>
+      <c r="H48" s="6"/>
+      <c r="I48" s="6">
+        <v>12</v>
+      </c>
+      <c r="J48" s="6"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A49" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B49" s="5">
+        <v>92.52</v>
+      </c>
+      <c r="C49" s="5">
+        <v>142.58000000000001</v>
+      </c>
+      <c r="D49" s="5">
+        <v>-310.06</v>
+      </c>
+      <c r="E49" s="5">
+        <v>-103.69</v>
+      </c>
+      <c r="F49" s="5">
+        <v>28.66</v>
+      </c>
+      <c r="G49" s="5">
+        <v>-8.0500000000000007</v>
+      </c>
+      <c r="H49" s="6"/>
+      <c r="I49" s="6">
+        <v>22</v>
+      </c>
+      <c r="J49" s="6"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A50" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B50" s="5">
+        <v>93.66</v>
+      </c>
+      <c r="C50" s="5">
+        <v>119.82</v>
+      </c>
+      <c r="D50" s="5">
+        <v>-280.17</v>
+      </c>
+      <c r="E50" s="5">
+        <v>-101.83</v>
+      </c>
+      <c r="F50" s="5">
+        <v>15.06</v>
+      </c>
+      <c r="G50" s="5">
+        <v>-23.92</v>
+      </c>
+      <c r="H50" s="6"/>
+      <c r="I50" s="6">
+        <v>23</v>
+      </c>
+      <c r="J50" s="6"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A51" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B51" s="7">
+        <v>98.59</v>
+      </c>
+      <c r="C51" s="7">
+        <v>104.19</v>
+      </c>
+      <c r="D51" s="7">
+        <v>-239.59</v>
+      </c>
+      <c r="E51" s="7">
+        <v>-87.51</v>
+      </c>
+      <c r="F51" s="7">
+        <v>32.020000000000003</v>
+      </c>
+      <c r="G51" s="7">
+        <v>23.89</v>
+      </c>
+      <c r="H51" s="8"/>
+      <c r="I51" s="8">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A18CD01-272C-E647-BB04-1ED24A3F1197}">
+  <dimension ref="A1:G33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:XFD45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5">
+        <v>-148.68</v>
+      </c>
+      <c r="C2" s="5">
+        <v>93.5</v>
+      </c>
+      <c r="D2" s="5">
+        <v>-133.16999999999999</v>
+      </c>
+      <c r="E2" s="5">
+        <v>-77.209999999999994</v>
+      </c>
+      <c r="F2" s="5">
+        <v>0.67</v>
+      </c>
+      <c r="G2" s="5">
+        <v>5.22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5">
+        <v>-136.71</v>
+      </c>
+      <c r="C3" s="5">
+        <v>62.2</v>
+      </c>
+      <c r="D3" s="5">
+        <v>-139.68</v>
+      </c>
+      <c r="E3" s="5">
+        <v>-172.53</v>
+      </c>
+      <c r="F3" s="5">
+        <v>-1.94</v>
+      </c>
+      <c r="G3" s="5">
+        <v>15.11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5">
+        <v>-111.26</v>
+      </c>
+      <c r="C4" s="5">
+        <v>25.89</v>
+      </c>
+      <c r="D4" s="5">
+        <v>-135.47999999999999</v>
+      </c>
+      <c r="E4" s="5">
+        <v>173.51</v>
+      </c>
+      <c r="F4" s="5">
+        <v>-19.100000000000001</v>
+      </c>
+      <c r="G4" s="5">
+        <v>23.12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5">
+        <v>70.14</v>
+      </c>
+      <c r="C5" s="5">
+        <v>-224.82</v>
+      </c>
+      <c r="D5" s="5">
+        <v>-149.83000000000001</v>
+      </c>
+      <c r="E5" s="5">
+        <v>62.09</v>
+      </c>
+      <c r="F5" s="5">
+        <v>-25.8</v>
+      </c>
+      <c r="G5" s="5">
+        <v>-20.58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5">
+        <v>76.08</v>
+      </c>
+      <c r="C6" s="5">
+        <v>-191.77</v>
+      </c>
+      <c r="D6" s="5">
+        <v>-150.53</v>
+      </c>
+      <c r="E6" s="5">
+        <v>6.23</v>
+      </c>
+      <c r="F6" s="5">
+        <v>-13.09</v>
+      </c>
+      <c r="G6" s="5">
+        <v>12.68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="6">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5">
+        <v>76.66</v>
+      </c>
+      <c r="C7" s="5">
+        <v>-146.81</v>
+      </c>
+      <c r="D7" s="5">
+        <v>-190.99</v>
+      </c>
+      <c r="E7" s="5">
+        <v>37.21</v>
+      </c>
+      <c r="F7" s="5">
+        <v>17.940000000000001</v>
+      </c>
+      <c r="G7" s="5">
+        <v>8.6199999999999992</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="6">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5">
+        <v>238.33</v>
+      </c>
+      <c r="C8" s="5">
+        <v>-31.44</v>
+      </c>
+      <c r="D8" s="5">
+        <v>-127.51</v>
+      </c>
+      <c r="E8" s="5">
+        <v>85.31</v>
+      </c>
+      <c r="F8" s="5">
+        <v>-34.950000000000003</v>
+      </c>
+      <c r="G8" s="5">
+        <v>9.15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="6">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5">
+        <v>216.7</v>
+      </c>
+      <c r="C9" s="5">
+        <v>-4.54</v>
+      </c>
+      <c r="D9" s="5">
+        <v>-132.74</v>
+      </c>
+      <c r="E9" s="5">
+        <v>12.38</v>
+      </c>
+      <c r="F9" s="5">
+        <v>-28.66</v>
+      </c>
+      <c r="G9" s="5">
+        <v>9.86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="6">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5">
+        <v>208.77</v>
+      </c>
+      <c r="C10" s="5">
+        <v>27.35</v>
+      </c>
+      <c r="D10" s="5">
+        <v>-123.77</v>
+      </c>
+      <c r="E10" s="5">
+        <v>25.46</v>
+      </c>
+      <c r="F10" s="5">
+        <v>-22.29</v>
+      </c>
+      <c r="G10" s="5">
+        <v>13.75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="6">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5">
+        <v>83.84</v>
+      </c>
+      <c r="C11" s="5">
+        <v>185.97</v>
+      </c>
+      <c r="D11" s="5">
+        <v>-151.76</v>
+      </c>
+      <c r="E11" s="5">
+        <v>-106.02</v>
+      </c>
+      <c r="F11" s="5">
+        <v>-15.39</v>
+      </c>
+      <c r="G11" s="5">
+        <v>7.12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="6">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5">
+        <v>73.69</v>
+      </c>
+      <c r="C12" s="5">
+        <v>163.27000000000001</v>
+      </c>
+      <c r="D12" s="5">
+        <v>-149.35</v>
+      </c>
+      <c r="E12" s="5">
+        <v>-48.95</v>
+      </c>
+      <c r="F12" s="5">
+        <v>-55.5</v>
+      </c>
+      <c r="G12" s="5">
+        <v>-15.03</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="6">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5">
+        <v>65.7</v>
+      </c>
+      <c r="C13" s="5">
+        <v>123.31</v>
+      </c>
+      <c r="D13" s="5">
+        <v>-164.55</v>
+      </c>
+      <c r="E13" s="5">
+        <v>-27.61</v>
+      </c>
+      <c r="F13" s="5">
+        <v>12.99</v>
+      </c>
+      <c r="G13" s="5">
+        <v>-19.37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="6">
+        <v>13</v>
+      </c>
+      <c r="B14" s="5">
+        <v>-183.67</v>
+      </c>
+      <c r="C14" s="5">
+        <v>48.72</v>
+      </c>
+      <c r="D14" s="5">
+        <v>-265.25</v>
+      </c>
+      <c r="E14" s="5">
+        <v>-39.49</v>
+      </c>
+      <c r="F14" s="5">
+        <v>22.08</v>
+      </c>
+      <c r="G14" s="5">
+        <v>-29.72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="6">
+        <v>14</v>
+      </c>
+      <c r="B15" s="5">
+        <v>-169.91</v>
+      </c>
+      <c r="C15" s="5">
+        <v>28.97</v>
+      </c>
+      <c r="D15" s="5">
+        <v>-261.47000000000003</v>
+      </c>
+      <c r="E15" s="5">
+        <v>55.1</v>
+      </c>
+      <c r="F15" s="5">
+        <v>26.44</v>
+      </c>
+      <c r="G15" s="5">
+        <v>-64.989999999999995</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="6">
+        <v>15</v>
+      </c>
+      <c r="B16" s="5">
+        <v>-157.80000000000001</v>
+      </c>
+      <c r="C16" s="5">
+        <v>11.3</v>
+      </c>
+      <c r="D16" s="5">
+        <v>-239.41</v>
+      </c>
+      <c r="E16" s="5">
+        <v>-46.93</v>
+      </c>
+      <c r="F16" s="5">
+        <v>21.62</v>
+      </c>
+      <c r="G16" s="5">
+        <v>-66.41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="6">
+        <v>16</v>
+      </c>
+      <c r="B17" s="5">
+        <v>67.16</v>
+      </c>
+      <c r="C17" s="5">
+        <v>-219.92</v>
+      </c>
+      <c r="D17" s="5">
+        <v>-302.11</v>
+      </c>
+      <c r="E17" s="5">
+        <v>61.3</v>
+      </c>
+      <c r="F17" s="5">
+        <v>-18.25</v>
+      </c>
+      <c r="G17" s="5">
+        <v>-3.52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="6">
+        <v>17</v>
+      </c>
+      <c r="B18" s="5">
+        <v>53.41</v>
+      </c>
+      <c r="C18" s="5">
+        <v>-208.55</v>
+      </c>
+      <c r="D18" s="5">
+        <v>-273.39999999999998</v>
+      </c>
+      <c r="E18" s="5">
+        <v>27.69</v>
+      </c>
+      <c r="F18" s="5">
+        <v>-4.13</v>
+      </c>
+      <c r="G18" s="5">
+        <v>38.74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="6">
+        <v>18</v>
+      </c>
+      <c r="B19" s="5">
+        <v>48.41</v>
+      </c>
+      <c r="C19" s="5">
+        <v>-179.83</v>
+      </c>
+      <c r="D19" s="5">
+        <v>-248.37</v>
+      </c>
+      <c r="E19" s="5">
+        <v>47.35</v>
+      </c>
+      <c r="F19" s="5">
+        <v>-10.16</v>
+      </c>
+      <c r="G19" s="5">
+        <v>53.29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="6">
+        <v>19</v>
+      </c>
+      <c r="B20" s="5">
+        <v>248.64</v>
+      </c>
+      <c r="C20" s="5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D20" s="5">
+        <v>-301.52999999999997</v>
+      </c>
+      <c r="E20" s="5">
+        <v>96.66</v>
+      </c>
+      <c r="F20" s="5">
+        <v>7.09</v>
+      </c>
+      <c r="G20" s="5">
+        <v>-21.65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="6">
+        <v>20</v>
+      </c>
+      <c r="B21" s="5">
+        <v>229.51</v>
+      </c>
+      <c r="C21" s="5">
+        <v>9.09</v>
+      </c>
+      <c r="D21" s="5">
+        <v>-281.70999999999998</v>
+      </c>
+      <c r="E21" s="5">
+        <v>60.22</v>
+      </c>
+      <c r="F21" s="5">
+        <v>37.81</v>
+      </c>
+      <c r="G21" s="5">
+        <v>28.51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="6">
+        <v>21</v>
+      </c>
+      <c r="B22" s="5">
+        <v>217.99</v>
+      </c>
+      <c r="C22" s="5">
+        <v>32.76</v>
+      </c>
+      <c r="D22" s="5">
+        <v>-251.13</v>
+      </c>
+      <c r="E22" s="5">
+        <v>87.09</v>
+      </c>
+      <c r="F22" s="5">
+        <v>10.65</v>
+      </c>
+      <c r="G22" s="5">
+        <v>50.39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="6">
+        <v>22</v>
+      </c>
+      <c r="B23" s="5">
+        <v>93.07</v>
+      </c>
+      <c r="C23" s="5">
+        <v>141.38</v>
+      </c>
+      <c r="D23" s="5">
+        <v>-311</v>
+      </c>
+      <c r="E23" s="5">
+        <v>-103.6</v>
+      </c>
+      <c r="F23" s="5">
+        <v>4.04</v>
+      </c>
+      <c r="G23" s="5">
+        <v>-75.38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="6">
+        <v>23</v>
+      </c>
+      <c r="B24" s="5">
+        <v>94.18</v>
+      </c>
+      <c r="C24" s="5">
+        <v>118.69</v>
+      </c>
+      <c r="D24" s="5">
+        <v>-279.89</v>
+      </c>
+      <c r="E24" s="5">
+        <v>-95.9</v>
+      </c>
+      <c r="F24" s="5">
+        <v>1.9</v>
+      </c>
+      <c r="G24" s="5">
+        <v>-89.9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="6">
+        <v>24</v>
+      </c>
+      <c r="B25" s="5">
+        <v>99.21</v>
+      </c>
+      <c r="C25" s="5">
+        <v>104.96</v>
+      </c>
+      <c r="D25" s="5">
+        <v>-239.65</v>
+      </c>
+      <c r="E25" s="5">
+        <v>-96.93</v>
+      </c>
+      <c r="F25" s="5">
+        <v>32</v>
+      </c>
+      <c r="G25" s="5">
+        <v>-3.63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="6">
+        <v>25</v>
+      </c>
+      <c r="B26" s="5">
+        <v>-22.27</v>
+      </c>
+      <c r="C26" s="5">
+        <v>-64.540000000000006</v>
+      </c>
+      <c r="D26" s="5">
+        <v>-347.43</v>
+      </c>
+      <c r="E26" s="5">
+        <v>-123.15</v>
+      </c>
+      <c r="F26" s="5">
+        <v>49.15</v>
+      </c>
+      <c r="G26" s="5">
+        <v>35.21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="6">
+        <v>26</v>
+      </c>
+      <c r="B27" s="5">
+        <v>26.39</v>
+      </c>
+      <c r="C27" s="5">
+        <v>-56.61</v>
+      </c>
+      <c r="D27" s="5">
+        <v>-332</v>
+      </c>
+      <c r="E27" s="5">
+        <v>-22.81</v>
+      </c>
+      <c r="F27" s="5">
+        <v>47.63</v>
+      </c>
+      <c r="G27" s="5">
+        <v>75.06</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="6">
+        <v>27</v>
+      </c>
+      <c r="B28" s="5">
+        <v>11.54</v>
+      </c>
+      <c r="C28" s="5">
+        <v>-116.62</v>
+      </c>
+      <c r="D28" s="5">
+        <v>-287.73</v>
+      </c>
+      <c r="E28" s="5">
+        <v>-78.83</v>
+      </c>
+      <c r="F28" s="5">
+        <v>32.49</v>
+      </c>
+      <c r="G28" s="5">
+        <v>67.95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="6">
+        <v>28</v>
+      </c>
+      <c r="B29" s="5">
+        <v>-46.53</v>
+      </c>
+      <c r="C29" s="5">
+        <v>-18.09</v>
+      </c>
+      <c r="D29" s="5">
+        <v>-265.7</v>
+      </c>
+      <c r="E29" s="5">
+        <v>52.35</v>
+      </c>
+      <c r="F29" s="5">
+        <v>6.85</v>
+      </c>
+      <c r="G29" s="5">
+        <v>5.86</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="6">
+        <v>29</v>
+      </c>
+      <c r="B30" s="5">
+        <v>-40.53</v>
+      </c>
+      <c r="C30" s="5">
+        <v>-86.38</v>
+      </c>
+      <c r="D30" s="5">
+        <v>-158.86000000000001</v>
+      </c>
+      <c r="E30" s="5">
+        <v>-76.25</v>
+      </c>
+      <c r="F30" s="5">
+        <v>-12.15</v>
+      </c>
+      <c r="G30" s="5">
+        <v>19.14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="6">
+        <v>30</v>
+      </c>
+      <c r="B31" s="5">
+        <v>55.85</v>
+      </c>
+      <c r="C31" s="5">
+        <v>-49.81</v>
+      </c>
+      <c r="D31" s="5">
+        <v>-150.11000000000001</v>
+      </c>
+      <c r="E31" s="5">
+        <v>-92.66</v>
+      </c>
+      <c r="F31" s="5">
+        <v>-1.79</v>
+      </c>
+      <c r="G31" s="5">
+        <v>-7.98</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="6">
+        <v>31</v>
+      </c>
+      <c r="B32" s="5">
+        <v>-27.09</v>
+      </c>
+      <c r="C32" s="5">
+        <v>-2.62</v>
+      </c>
+      <c r="D32" s="5">
+        <v>-83.24</v>
+      </c>
+      <c r="E32" s="5">
+        <v>-61.45</v>
+      </c>
+      <c r="F32" s="5">
+        <v>-2.58</v>
+      </c>
+      <c r="G32" s="5">
+        <v>7.08</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="6">
+        <v>32</v>
+      </c>
+      <c r="B33" s="5">
+        <v>117.51</v>
+      </c>
+      <c r="C33" s="5">
+        <v>74.08</v>
+      </c>
+      <c r="D33" s="5">
+        <v>-147.46</v>
+      </c>
+      <c r="E33" s="5">
+        <v>-18.75</v>
+      </c>
+      <c r="F33" s="5">
+        <v>1.48</v>
+      </c>
+      <c r="G33" s="5">
+        <v>-6.03</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>